<commit_message>
added sort site parser and xlsx writer
</commit_message>
<xml_diff>
--- a/logs/test_log_contrast.xlsx
+++ b/logs/test_log_contrast.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>background_color</t>
   </si>
@@ -31,31 +31,22 @@
     <t>fix_remarks</t>
   </si>
   <si>
-    <t>HEX: #04aa6d</t>
-  </si>
-  <si>
     <t>HEX: #ffffff</t>
   </si>
   <si>
-    <t>&lt;a id="w3loginbtn" class="w3-bar-item w3-btn bar-item-hover w3-right" style="display: inline; width: 130px; background-color: rgb(4, 170, 109); color: white; border-radius: 25px;" href="https://profil</t>
-  </si>
-  <si>
-    <t>3.01:1</t>
-  </si>
-  <si>
-    <t>Increase contrast by at least 49.5% to pass.</t>
-  </si>
-  <si>
-    <t>HEX: #ff0000</t>
-  </si>
-  <si>
-    <t>&lt;span class="pythonnumbercolor" style="color:red"&gt;1&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>3.99:1</t>
-  </si>
-  <si>
-    <t>Increase contrast by at least 12.78% to pass.</t>
+    <t>&lt;a class="color-link" href="/?themecolor=default"&gt;.&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>Increase contrast by at least 350% to pass.</t>
+  </si>
+  <si>
+    <t>HEX: #000000</t>
+  </si>
+  <si>
+    <t>&lt;a class="color-link" href="/?themecolor=blacktheme"&gt;.&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -415,33 +406,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>